<commit_message>
add us in location.json
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="246">
   <si>
     <t>ID</t>
   </si>
@@ -808,6 +808,14 @@
   </si>
   <si>
     <t>State</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>US</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>只设置US可取消location限制</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1738,10 +1746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -2696,6 +2704,14 @@
       </c>
       <c r="H51" s="2" t="s">
         <v>186</v>
+      </c>
+    </row>
+    <row r="52" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E52" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>